<commit_message>
Ready for Multi Thread and Events Proramming
</commit_message>
<xml_diff>
--- a/工作簿1.xlsx
+++ b/工作簿1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18424"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>班级</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,10 +34,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -46,47 +42,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>大小周</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>学部</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Class1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cambridge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学生1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A方向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学生1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A方</t>
+    <t>刘浩宇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘壮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李沚璠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谭一诺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沧州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>廊坊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沧州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任丘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>韩蓝颖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李月童</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初三十班</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初中部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>崔兆言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>万宇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沧州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李大千</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张家口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张鹏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张家口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +137,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -129,13 +177,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -451,84 +499,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="14.875" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>200</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+    </row>
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Encrypted And something ELSE inportant
</commit_message>
<xml_diff>
--- a/工作簿1.xlsx
+++ b/工作簿1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\YH-SchoolBus-WoodenBench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WoodenBench for Schoolbus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="19">
   <si>
     <t>班级</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,22 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>沧州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>廊坊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>沧州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>任丘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>韩蓝颖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -102,20 +86,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>沧州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>李大千</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>张家口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>张鹏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>张畔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沧州-青县</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贾雨昂</t>
   </si>
 </sst>
 </file>
@@ -169,14 +152,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -496,132 +482,812 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="14.875" style="2"/>
+    <col min="1" max="16384" width="14.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B31" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B39" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B40" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B43" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B44" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
+      <c r="B47" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nearly Finished Database Connection.....
Bug: If too much load, Database Server will send currupted data and in wrong sequence,,
</commit_message>
<xml_diff>
--- a/工作簿1.xlsx
+++ b/工作簿1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WoodenBench for Schoolbus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SchoolBus_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E797BE-B9BC-4339-BE45-2C99252B3947}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>班级</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -484,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -619,676 +620,270 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
     </row>
     <row r="37" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B40" s="3"/>
     </row>
     <row r="41" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B44" s="3"/>
     </row>
     <row r="45" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
     </row>
     <row r="48" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B48" s="3"/>
     </row>
     <row r="49" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B49" s="3"/>
     </row>
     <row r="50" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B50" s="3"/>
     </row>
     <row r="51" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B51" s="3"/>
     </row>
     <row r="52" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B52" s="3"/>
     </row>
     <row r="53" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B53" s="3"/>
     </row>
     <row r="54" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B55" s="3"/>
     </row>
     <row r="56" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
     </row>
     <row r="58" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
     </row>
     <row r="59" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B59" s="3"/>
     </row>
     <row r="60" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B60" s="3"/>
     </row>
     <row r="61" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B61" s="3"/>
     </row>
     <row r="62" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B63" s="3"/>
     </row>
     <row r="64" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B64" s="3"/>
     </row>
     <row r="65" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B66" s="3"/>
     </row>
     <row r="67" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B70" s="3"/>
     </row>
     <row r="71" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B72" s="3"/>
     </row>
     <row r="73" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B77" s="3"/>
     </row>
     <row r="78" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
     </row>
     <row r="80" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B88" s="3"/>
     </row>
     <row r="89" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B89" s="3"/>
     </row>
     <row r="90" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
     </row>
     <row r="91" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B92" s="3"/>
     </row>
     <row r="93" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B93" s="3"/>
     </row>
     <row r="94" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B94" s="3"/>
     </row>
     <row r="95" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>